<commit_message>
RSNN uniform files to be run
</commit_message>
<xml_diff>
--- a/SHDFinal/FeedForwardSNN/Training-TestAccuracies.xlsx
+++ b/SHDFinal/FeedForwardSNN/Training-TestAccuracies.xlsx
@@ -87,10 +87,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -403,7 +403,7 @@
   <dimension ref="B4:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,12 +412,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -439,10 +439,10 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>200</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="5">
         <v>400</v>
       </c>
@@ -461,6 +461,12 @@
       <c r="F7">
         <v>0.46400000000000002</v>
       </c>
+      <c r="G7">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.51100000000000001</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D8">
@@ -472,6 +478,12 @@
       <c r="F8">
         <v>0.55200000000000005</v>
       </c>
+      <c r="G8">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H8">
+        <v>0.55400000000000005</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
@@ -486,6 +498,12 @@
       <c r="F10">
         <v>0.48499999999999999</v>
       </c>
+      <c r="G10">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="H10">
+        <v>0.55300000000000005</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D11">
@@ -496,6 +514,12 @@
       </c>
       <c r="F11">
         <v>0.60599999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="H11">
+        <v>0.60299999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>